<commit_message>
Local storage keys now use names instead of indices, to allow items to be reordered in the spreadsheet
</commit_message>
<xml_diff>
--- a/public/games/powerwashsimulator/powerwashsimulator_data.xlsx
+++ b/public/games/powerwashsimulator/powerwashsimulator_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\Achievement-Vault\public\games\powerwashsimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CD5025-6202-4B01-B1E3-9D577253F4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCF9BDF-D74D-43B3-94D0-C1D90E300AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="900" windowWidth="21825" windowHeight="14190" xr2:uid="{30C4C3A8-F402-46FC-A1A0-0B0F8647869F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30C4C3A8-F402-46FC-A1A0-0B0F8647869F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -723,14 +723,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,13 +1067,15 @@
   <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+      <selection activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="25" max="25" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="47.25" x14ac:dyDescent="0.25">
@@ -1236,13 +1237,16 @@
       <c r="X2">
         <v>1</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="3" t="s">
         <v>190</v>
       </c>
       <c r="Z2" t="s">
         <v>191</v>
       </c>
       <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
         <v>1</v>
       </c>
     </row>
@@ -1319,13 +1323,16 @@
       <c r="X3">
         <v>1</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Y3" s="3" t="s">
         <v>192</v>
       </c>
       <c r="Z3" t="s">
         <v>193</v>
       </c>
       <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
         <v>1</v>
       </c>
     </row>
@@ -1402,13 +1409,16 @@
       <c r="X4">
         <v>1</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" s="3" t="s">
         <v>194</v>
       </c>
       <c r="Z4" t="s">
         <v>195</v>
       </c>
       <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
         <v>1</v>
       </c>
     </row>
@@ -1485,7 +1495,7 @@
       <c r="X5">
         <v>1</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Y5" t="s">
         <v>196</v>
       </c>
       <c r="Z5" t="s">
@@ -1568,7 +1578,7 @@
       <c r="X6">
         <v>1</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Y6" t="s">
         <v>198</v>
       </c>
       <c r="Z6" t="s">
@@ -1651,13 +1661,16 @@
       <c r="X7">
         <v>1</v>
       </c>
-      <c r="Y7" s="4" t="s">
+      <c r="Y7" s="3" t="s">
         <v>200</v>
       </c>
       <c r="Z7" t="s">
         <v>201</v>
       </c>
       <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
         <v>1</v>
       </c>
     </row>
@@ -1734,13 +1747,16 @@
       <c r="X8">
         <v>1</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="Y8" s="3" t="s">
         <v>202</v>
       </c>
       <c r="Z8" t="s">
         <v>203</v>
       </c>
       <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
         <v>1</v>
       </c>
     </row>
@@ -1817,13 +1833,16 @@
       <c r="X9">
         <v>1</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="Y9" s="3" t="s">
         <v>204</v>
       </c>
       <c r="Z9" t="s">
         <v>205</v>
       </c>
       <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
         <v>1</v>
       </c>
     </row>
@@ -1900,7 +1919,7 @@
       <c r="X10">
         <v>1</v>
       </c>
-      <c r="Y10" s="4" t="s">
+      <c r="Y10" t="s">
         <v>206</v>
       </c>
       <c r="Z10" t="s">
@@ -1983,7 +2002,7 @@
       <c r="X11">
         <v>1</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="Y11" t="s">
         <v>208</v>
       </c>
       <c r="Z11" t="s">

</xml_diff>